<commit_message>
Updated SLBS Manual Major Project
</commit_message>
<xml_diff>
--- a/MAJOR_MANUAL_PROJECT.xlsx
+++ b/MAJOR_MANUAL_PROJECT.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo\Desktop\SOFTWARE_TESTING\MAJOR_PROJECT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DE591E6-7D53-4FE3-8577-0C4EA7C77FF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55CC28D4-8778-4FE4-8601-67872F93ABBB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="10380" activeTab="2" xr2:uid="{45127632-98AF-42C8-B62A-A8E061A445F9}"/>
+    <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="10380" xr2:uid="{45127632-98AF-42C8-B62A-A8E061A445F9}"/>
   </bookViews>
   <sheets>
     <sheet name="Test_Cases" sheetId="1" r:id="rId1"/>
@@ -1324,17 +1324,17 @@
     <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -3933,12 +3933,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F06B50AF-DC18-4739-A5F9-E04F19DCE45A}">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:G69"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A56" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G2" sqref="G1:G1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" sqref="A1:G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
@@ -3953,15 +3952,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="19" x14ac:dyDescent="0.95">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="21"/>
-      <c r="C1" s="21"/>
-      <c r="D1" s="21"/>
-      <c r="E1" s="21"/>
-      <c r="F1" s="21"/>
-      <c r="G1" s="21"/>
+      <c r="B1" s="23"/>
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
+      <c r="F1" s="23"/>
+      <c r="G1" s="23"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A2" s="1" t="s">
@@ -4017,17 +4016,17 @@
       </c>
     </row>
     <row r="5" spans="1:7" s="9" customFormat="1" x14ac:dyDescent="0.75">
-      <c r="A5" s="20" t="s">
+      <c r="A5" s="22" t="s">
         <v>108</v>
       </c>
-      <c r="B5" s="20"/>
-      <c r="C5" s="20"/>
-      <c r="D5" s="20"/>
-      <c r="E5" s="20"/>
-      <c r="F5" s="20"/>
-      <c r="G5" s="20"/>
-    </row>
-    <row r="6" spans="1:7" s="9" customFormat="1" ht="29.5" hidden="1" x14ac:dyDescent="0.75">
+      <c r="B5" s="22"/>
+      <c r="C5" s="22"/>
+      <c r="D5" s="22"/>
+      <c r="E5" s="22"/>
+      <c r="F5" s="22"/>
+      <c r="G5" s="22"/>
+    </row>
+    <row r="6" spans="1:7" s="9" customFormat="1" ht="29.5" x14ac:dyDescent="0.75">
       <c r="A6" s="9" t="s">
         <v>13</v>
       </c>
@@ -4050,7 +4049,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="7" spans="1:7" s="9" customFormat="1" ht="29.5" hidden="1" x14ac:dyDescent="0.75">
+    <row r="7" spans="1:7" s="9" customFormat="1" ht="29.5" x14ac:dyDescent="0.75">
       <c r="A7" s="9" t="s">
         <v>14</v>
       </c>
@@ -4073,7 +4072,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="8" spans="1:7" s="9" customFormat="1" ht="29.5" hidden="1" x14ac:dyDescent="0.75">
+    <row r="8" spans="1:7" s="9" customFormat="1" ht="29.5" x14ac:dyDescent="0.75">
       <c r="A8" s="9" t="s">
         <v>15</v>
       </c>
@@ -4096,7 +4095,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="9" spans="1:7" s="10" customFormat="1" ht="88.5" hidden="1" x14ac:dyDescent="0.75">
+    <row r="9" spans="1:7" s="10" customFormat="1" ht="88.5" x14ac:dyDescent="0.75">
       <c r="A9" s="10" t="s">
         <v>16</v>
       </c>
@@ -4142,7 +4141,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="11" spans="1:7" s="9" customFormat="1" ht="29.5" hidden="1" x14ac:dyDescent="0.75">
+    <row r="11" spans="1:7" s="9" customFormat="1" ht="29.5" x14ac:dyDescent="0.75">
       <c r="A11" s="9" t="s">
         <v>18</v>
       </c>
@@ -4165,7 +4164,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="12" spans="1:7" s="9" customFormat="1" ht="29.5" hidden="1" x14ac:dyDescent="0.75">
+    <row r="12" spans="1:7" s="9" customFormat="1" ht="29.5" x14ac:dyDescent="0.75">
       <c r="A12" s="9" t="s">
         <v>19</v>
       </c>
@@ -4188,7 +4187,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="13" spans="1:7" s="9" customFormat="1" ht="29.5" hidden="1" x14ac:dyDescent="0.75">
+    <row r="13" spans="1:7" s="9" customFormat="1" ht="29.5" x14ac:dyDescent="0.75">
       <c r="A13" s="9" t="s">
         <v>20</v>
       </c>
@@ -4211,7 +4210,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="14" spans="1:7" s="9" customFormat="1" ht="29.5" hidden="1" x14ac:dyDescent="0.75">
+    <row r="14" spans="1:7" s="9" customFormat="1" ht="29.5" x14ac:dyDescent="0.75">
       <c r="A14" s="9" t="s">
         <v>21</v>
       </c>
@@ -4280,7 +4279,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="17" spans="1:7" s="9" customFormat="1" ht="162.25" hidden="1" x14ac:dyDescent="0.75">
+    <row r="17" spans="1:7" s="9" customFormat="1" ht="162.25" x14ac:dyDescent="0.75">
       <c r="A17" s="9" t="s">
         <v>24</v>
       </c>
@@ -4303,7 +4302,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="18" spans="1:7" s="9" customFormat="1" ht="147.5" hidden="1" x14ac:dyDescent="0.75">
+    <row r="18" spans="1:7" s="9" customFormat="1" ht="147.5" x14ac:dyDescent="0.75">
       <c r="A18" s="9" t="s">
         <v>72</v>
       </c>
@@ -4349,7 +4348,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="20" spans="1:7" s="9" customFormat="1" ht="29.5" hidden="1" x14ac:dyDescent="0.75">
+    <row r="20" spans="1:7" s="9" customFormat="1" ht="29.5" x14ac:dyDescent="0.75">
       <c r="A20" s="9" t="s">
         <v>74</v>
       </c>
@@ -4395,7 +4394,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="22" spans="1:7" s="9" customFormat="1" ht="29.5" hidden="1" x14ac:dyDescent="0.75">
+    <row r="22" spans="1:7" s="9" customFormat="1" ht="29.5" x14ac:dyDescent="0.75">
       <c r="A22" s="9" t="s">
         <v>76</v>
       </c>
@@ -4418,7 +4417,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="23" spans="1:7" s="9" customFormat="1" ht="29.5" hidden="1" x14ac:dyDescent="0.75">
+    <row r="23" spans="1:7" s="9" customFormat="1" ht="29.5" x14ac:dyDescent="0.75">
       <c r="A23" s="9" t="s">
         <v>77</v>
       </c>
@@ -4464,7 +4463,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="25" spans="1:7" s="9" customFormat="1" ht="44.25" hidden="1" x14ac:dyDescent="0.75">
+    <row r="25" spans="1:7" s="9" customFormat="1" ht="44.25" x14ac:dyDescent="0.75">
       <c r="A25" s="9" t="s">
         <v>103</v>
       </c>
@@ -4487,7 +4486,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="26" spans="1:7" s="9" customFormat="1" ht="29.5" hidden="1" x14ac:dyDescent="0.75">
+    <row r="26" spans="1:7" s="9" customFormat="1" ht="29.5" x14ac:dyDescent="0.75">
       <c r="A26" s="9" t="s">
         <v>110</v>
       </c>
@@ -4511,17 +4510,17 @@
       </c>
     </row>
     <row r="27" spans="1:7" s="9" customFormat="1" x14ac:dyDescent="0.75">
-      <c r="A27" s="20" t="s">
+      <c r="A27" s="22" t="s">
         <v>109</v>
       </c>
-      <c r="B27" s="20"/>
-      <c r="C27" s="20"/>
-      <c r="D27" s="20"/>
-      <c r="E27" s="20"/>
-      <c r="F27" s="20"/>
-      <c r="G27" s="20"/>
-    </row>
-    <row r="28" spans="1:7" s="9" customFormat="1" ht="29.5" hidden="1" x14ac:dyDescent="0.75">
+      <c r="B27" s="22"/>
+      <c r="C27" s="22"/>
+      <c r="D27" s="22"/>
+      <c r="E27" s="22"/>
+      <c r="F27" s="22"/>
+      <c r="G27" s="22"/>
+    </row>
+    <row r="28" spans="1:7" s="9" customFormat="1" ht="29.5" x14ac:dyDescent="0.75">
       <c r="A28" s="9" t="s">
         <v>111</v>
       </c>
@@ -4567,7 +4566,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="30" spans="1:7" s="9" customFormat="1" ht="44.25" hidden="1" x14ac:dyDescent="0.75">
+    <row r="30" spans="1:7" s="9" customFormat="1" ht="44.25" x14ac:dyDescent="0.75">
       <c r="A30" s="9" t="s">
         <v>113</v>
       </c>
@@ -4614,17 +4613,17 @@
       </c>
     </row>
     <row r="32" spans="1:7" s="9" customFormat="1" x14ac:dyDescent="0.75">
-      <c r="A32" s="20" t="s">
+      <c r="A32" s="22" t="s">
         <v>131</v>
       </c>
-      <c r="B32" s="20"/>
-      <c r="C32" s="20"/>
-      <c r="D32" s="20"/>
-      <c r="E32" s="20"/>
-      <c r="F32" s="20"/>
-      <c r="G32" s="20"/>
-    </row>
-    <row r="33" spans="1:7" s="9" customFormat="1" ht="29.5" hidden="1" x14ac:dyDescent="0.75">
+      <c r="B32" s="22"/>
+      <c r="C32" s="22"/>
+      <c r="D32" s="22"/>
+      <c r="E32" s="22"/>
+      <c r="F32" s="22"/>
+      <c r="G32" s="22"/>
+    </row>
+    <row r="33" spans="1:7" s="9" customFormat="1" ht="29.5" x14ac:dyDescent="0.75">
       <c r="A33" s="9" t="s">
         <v>137</v>
       </c>
@@ -4694,17 +4693,17 @@
       </c>
     </row>
     <row r="36" spans="1:7" s="9" customFormat="1" x14ac:dyDescent="0.75">
-      <c r="A36" s="20" t="s">
+      <c r="A36" s="22" t="s">
         <v>143</v>
       </c>
-      <c r="B36" s="20"/>
-      <c r="C36" s="20"/>
-      <c r="D36" s="20"/>
-      <c r="E36" s="20"/>
-      <c r="F36" s="20"/>
-      <c r="G36" s="20"/>
-    </row>
-    <row r="37" spans="1:7" s="9" customFormat="1" ht="29.5" hidden="1" x14ac:dyDescent="0.75">
+      <c r="B36" s="22"/>
+      <c r="C36" s="22"/>
+      <c r="D36" s="22"/>
+      <c r="E36" s="22"/>
+      <c r="F36" s="22"/>
+      <c r="G36" s="22"/>
+    </row>
+    <row r="37" spans="1:7" s="9" customFormat="1" ht="29.5" x14ac:dyDescent="0.75">
       <c r="A37" s="9" t="s">
         <v>146</v>
       </c>
@@ -4750,7 +4749,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="39" spans="1:7" s="9" customFormat="1" hidden="1" x14ac:dyDescent="0.75">
+    <row r="39" spans="1:7" s="9" customFormat="1" x14ac:dyDescent="0.75">
       <c r="A39" s="9" t="s">
         <v>150</v>
       </c>
@@ -4773,7 +4772,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="40" spans="1:7" s="9" customFormat="1" ht="29.5" hidden="1" x14ac:dyDescent="0.75">
+    <row r="40" spans="1:7" s="9" customFormat="1" ht="29.5" x14ac:dyDescent="0.75">
       <c r="A40" s="9" t="s">
         <v>154</v>
       </c>
@@ -4797,17 +4796,17 @@
       </c>
     </row>
     <row r="41" spans="1:7" s="9" customFormat="1" x14ac:dyDescent="0.75">
-      <c r="A41" s="20" t="s">
+      <c r="A41" s="22" t="s">
         <v>153</v>
       </c>
-      <c r="B41" s="20"/>
-      <c r="C41" s="20"/>
-      <c r="D41" s="20"/>
-      <c r="E41" s="20"/>
-      <c r="F41" s="20"/>
-      <c r="G41" s="20"/>
-    </row>
-    <row r="42" spans="1:7" s="9" customFormat="1" ht="29.5" hidden="1" x14ac:dyDescent="0.75">
+      <c r="B41" s="22"/>
+      <c r="C41" s="22"/>
+      <c r="D41" s="22"/>
+      <c r="E41" s="22"/>
+      <c r="F41" s="22"/>
+      <c r="G41" s="22"/>
+    </row>
+    <row r="42" spans="1:7" s="9" customFormat="1" ht="29.5" x14ac:dyDescent="0.75">
       <c r="A42" s="9" t="s">
         <v>158</v>
       </c>
@@ -4853,7 +4852,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="44" spans="1:7" s="9" customFormat="1" ht="132.75" hidden="1" x14ac:dyDescent="0.75">
+    <row r="44" spans="1:7" s="9" customFormat="1" ht="132.75" x14ac:dyDescent="0.75">
       <c r="A44" s="9" t="s">
         <v>163</v>
       </c>
@@ -4876,7 +4875,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="45" spans="1:7" s="9" customFormat="1" ht="73.75" hidden="1" x14ac:dyDescent="0.75">
+    <row r="45" spans="1:7" s="9" customFormat="1" ht="73.75" x14ac:dyDescent="0.75">
       <c r="A45" s="9" t="s">
         <v>167</v>
       </c>
@@ -4899,7 +4898,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="46" spans="1:7" s="9" customFormat="1" ht="29.5" hidden="1" x14ac:dyDescent="0.75">
+    <row r="46" spans="1:7" s="9" customFormat="1" ht="29.5" x14ac:dyDescent="0.75">
       <c r="A46" s="9" t="s">
         <v>173</v>
       </c>
@@ -4945,7 +4944,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="48" spans="1:7" s="9" customFormat="1" ht="29.5" hidden="1" x14ac:dyDescent="0.75">
+    <row r="48" spans="1:7" s="9" customFormat="1" ht="29.5" x14ac:dyDescent="0.75">
       <c r="A48" s="9" t="s">
         <v>181</v>
       </c>
@@ -4991,7 +4990,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="50" spans="1:7" s="9" customFormat="1" ht="29.5" hidden="1" x14ac:dyDescent="0.75">
+    <row r="50" spans="1:7" s="9" customFormat="1" ht="29.5" x14ac:dyDescent="0.75">
       <c r="A50" s="9" t="s">
         <v>193</v>
       </c>
@@ -5014,7 +5013,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="51" spans="1:7" s="9" customFormat="1" ht="29.5" hidden="1" x14ac:dyDescent="0.75">
+    <row r="51" spans="1:7" s="9" customFormat="1" ht="29.5" x14ac:dyDescent="0.75">
       <c r="A51" s="9" t="s">
         <v>199</v>
       </c>
@@ -5060,7 +5059,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="53" spans="1:7" s="9" customFormat="1" ht="29.5" hidden="1" x14ac:dyDescent="0.75">
+    <row r="53" spans="1:7" s="9" customFormat="1" ht="29.5" x14ac:dyDescent="0.75">
       <c r="A53" s="9" t="s">
         <v>211</v>
       </c>
@@ -5083,7 +5082,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="54" spans="1:7" s="9" customFormat="1" ht="59" hidden="1" x14ac:dyDescent="0.75">
+    <row r="54" spans="1:7" s="9" customFormat="1" ht="59" x14ac:dyDescent="0.75">
       <c r="A54" s="9" t="s">
         <v>216</v>
       </c>
@@ -5106,7 +5105,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="55" spans="1:7" s="9" customFormat="1" ht="44.25" hidden="1" x14ac:dyDescent="0.75">
+    <row r="55" spans="1:7" s="9" customFormat="1" ht="44.25" x14ac:dyDescent="0.75">
       <c r="A55" s="9" t="s">
         <v>222</v>
       </c>
@@ -5199,17 +5198,17 @@
       </c>
     </row>
     <row r="59" spans="1:7" s="9" customFormat="1" x14ac:dyDescent="0.75">
-      <c r="A59" s="20" t="s">
+      <c r="A59" s="22" t="s">
         <v>241</v>
       </c>
-      <c r="B59" s="20"/>
-      <c r="C59" s="20"/>
-      <c r="D59" s="20"/>
-      <c r="E59" s="20"/>
-      <c r="F59" s="20"/>
-      <c r="G59" s="20"/>
-    </row>
-    <row r="60" spans="1:7" s="9" customFormat="1" ht="29.5" hidden="1" x14ac:dyDescent="0.75">
+      <c r="B59" s="22"/>
+      <c r="C59" s="22"/>
+      <c r="D59" s="22"/>
+      <c r="E59" s="22"/>
+      <c r="F59" s="22"/>
+      <c r="G59" s="22"/>
+    </row>
+    <row r="60" spans="1:7" s="9" customFormat="1" ht="29.5" x14ac:dyDescent="0.75">
       <c r="A60" s="9" t="s">
         <v>242</v>
       </c>
@@ -5232,7 +5231,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="61" spans="1:7" s="9" customFormat="1" ht="29.5" hidden="1" x14ac:dyDescent="0.75">
+    <row r="61" spans="1:7" s="9" customFormat="1" ht="29.5" x14ac:dyDescent="0.75">
       <c r="A61" s="9" t="s">
         <v>247</v>
       </c>
@@ -5278,7 +5277,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="63" spans="1:7" s="9" customFormat="1" ht="29.5" hidden="1" x14ac:dyDescent="0.75">
+    <row r="63" spans="1:7" s="9" customFormat="1" ht="29.5" x14ac:dyDescent="0.75">
       <c r="A63" s="9" t="s">
         <v>255</v>
       </c>
@@ -5301,7 +5300,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="64" spans="1:7" s="9" customFormat="1" ht="29.5" hidden="1" x14ac:dyDescent="0.75">
+    <row r="64" spans="1:7" s="9" customFormat="1" ht="29.5" x14ac:dyDescent="0.75">
       <c r="A64" s="9" t="s">
         <v>258</v>
       </c>
@@ -5324,7 +5323,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="65" spans="1:7" s="9" customFormat="1" ht="29.5" hidden="1" x14ac:dyDescent="0.75">
+    <row r="65" spans="1:7" s="9" customFormat="1" ht="29.5" x14ac:dyDescent="0.75">
       <c r="A65" s="9" t="s">
         <v>264</v>
       </c>
@@ -5393,7 +5392,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="68" spans="1:7" s="9" customFormat="1" ht="29.5" hidden="1" x14ac:dyDescent="0.75">
+    <row r="68" spans="1:7" s="9" customFormat="1" ht="29.5" x14ac:dyDescent="0.75">
       <c r="A68" s="9" t="s">
         <v>277</v>
       </c>
@@ -5416,7 +5415,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="69" spans="1:7" s="9" customFormat="1" ht="44.25" hidden="1" x14ac:dyDescent="0.75">
+    <row r="69" spans="1:7" s="9" customFormat="1" ht="44.25" x14ac:dyDescent="0.75">
       <c r="A69" s="9" t="s">
         <v>282</v>
       </c>
@@ -5440,13 +5439,6 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A4:G69" xr:uid="{F06B50AF-DC18-4739-A5F9-E04F19DCE45A}">
-    <filterColumn colId="6">
-      <filters blank="1">
-        <filter val="Fail"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
   <mergeCells count="7">
     <mergeCell ref="A41:G41"/>
     <mergeCell ref="A59:G59"/>
@@ -5523,9 +5515,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FAF127E4-B6C2-45A7-BB6C-FDC002C9D885}">
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L10" sqref="L10"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
   <cols>
@@ -5619,7 +5609,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3BC64513-5E6F-441D-8D4C-DF03248201C3}">
   <dimension ref="A1:I25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:I1"/>
     </sheetView>
   </sheetViews>
@@ -5637,17 +5627,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="19" x14ac:dyDescent="0.95">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="21"/>
-      <c r="C1" s="21"/>
-      <c r="D1" s="21"/>
-      <c r="E1" s="21"/>
-      <c r="F1" s="21"/>
-      <c r="G1" s="21"/>
-      <c r="H1" s="21"/>
-      <c r="I1" s="21"/>
+      <c r="B1" s="23"/>
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
+      <c r="F1" s="23"/>
+      <c r="G1" s="23"/>
+      <c r="H1" s="23"/>
+      <c r="I1" s="23"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.75">
       <c r="A2" s="1" t="s">
@@ -5657,7 +5647,7 @@
       <c r="C2" s="4"/>
       <c r="D2" s="4"/>
       <c r="E2" s="6"/>
-      <c r="F2" s="22"/>
+      <c r="F2" s="20"/>
       <c r="G2" s="1"/>
       <c r="H2" s="1" t="s">
         <v>10</v>
@@ -5674,7 +5664,7 @@
       <c r="C3" s="4"/>
       <c r="D3" s="4"/>
       <c r="E3" s="6"/>
-      <c r="F3" s="23"/>
+      <c r="F3" s="21"/>
       <c r="G3" s="1"/>
       <c r="H3" s="1" t="s">
         <v>11</v>

</xml_diff>